<commit_message>
Updated README file and removed runtime output data from .ipynb file
</commit_message>
<xml_diff>
--- a/Qsim-CPU/Amplitude-Estimation/Amplitude Estimation Benchmark-Results.xlsx
+++ b/Qsim-CPU/Amplitude-Estimation/Amplitude Estimation Benchmark-Results.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1209,570 +1209,1231 @@
       <c r="T18" s="1" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>Number of Qubits</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="1" t="inlineStr">
         <is>
           <t>avg_creation_times (ms)</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="1" t="inlineStr">
         <is>
           <t>std_creation_times (ms)</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="1" t="inlineStr">
         <is>
           <t>avg_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" s="1" t="inlineStr">
         <is>
           <t>std_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="1" t="inlineStr">
         <is>
           <t>avg_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" s="1" t="inlineStr">
         <is>
           <t>std_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H19" s="1" t="inlineStr">
         <is>
           <t>avg_circuit_depths</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" s="1" t="inlineStr">
         <is>
           <t>avg_transpiled_depths</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J19" s="1" t="inlineStr">
         <is>
           <t>Average_Rescaled_fidelity</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="K19" s="1" t="inlineStr">
         <is>
           <t>Average_Hellinger_fidelity</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="L19" s="1" t="inlineStr">
         <is>
           <t>std_Rescaled_Fidelity</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M19" s="1" t="inlineStr">
         <is>
           <t>std_hellinger_fidelity</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="N19" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="O19" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="P19" s="1" t="inlineStr">
         <is>
           <t>avg_xi (n2q/n1q+n2q)</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="Q19" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="R19" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
+      <c r="S19" s="1" t="inlineStr">
         <is>
           <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
         </is>
       </c>
-      <c r="T19" t="inlineStr">
+      <c r="T19" s="1" t="inlineStr">
         <is>
           <t>max_memory (MB)</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="1" t="n">
         <v>6.736</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="1" t="n">
         <v>0.111</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="1" t="n">
         <v>183.193</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="1" t="n">
         <v>10.269</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20" s="1" t="n">
         <v>20.919</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" s="1" t="n">
         <v>0.353</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" s="1" t="n">
         <v>167.5</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="K20" t="n">
+      <c r="K20" s="1" t="n">
         <v>0.27</v>
       </c>
-      <c r="L20" t="n">
+      <c r="L20" s="1" t="n">
         <v>0.017</v>
       </c>
-      <c r="M20" t="n">
+      <c r="M20" s="1" t="n">
         <v>0.018</v>
       </c>
-      <c r="N20" t="n">
+      <c r="N20" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="O20" t="n">
+      <c r="O20" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="P20" t="n">
+      <c r="P20" s="1" t="n">
         <v>0.63</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="Q20" s="1" t="n">
         <v>128.5</v>
       </c>
-      <c r="R20" t="n">
+      <c r="R20" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="S20" t="n">
+      <c r="S20" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="T20" t="n">
+      <c r="T20" s="1" t="n">
         <v>170.08</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="1" t="n">
         <v>8.538</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="1" t="n">
         <v>0.012</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="1" t="n">
         <v>414.781</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="1" t="n">
         <v>0.732</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21" s="1" t="n">
         <v>119.168</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21" s="1" t="n">
         <v>0.151</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="1" t="n">
         <v>479</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" s="1" t="n">
         <v>363</v>
       </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
+      <c r="J21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1" t="n">
         <v>0.19</v>
       </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
+      <c r="L21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="O21" t="n">
+      <c r="O21" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="P21" t="n">
+      <c r="P21" s="1" t="n">
         <v>0.65</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="Q21" s="1" t="n">
         <v>277</v>
       </c>
-      <c r="R21" t="n">
+      <c r="R21" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="S21" t="n">
+      <c r="S21" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="T21" t="n">
+      <c r="T21" s="1" t="n">
         <v>171.42</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" s="1" t="n">
         <v>12.626</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="1" t="n">
         <v>0.006</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="1" t="n">
         <v>1507.784</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" s="1" t="n">
         <v>3.411</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22" s="1" t="n">
         <v>957.63</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22" s="1" t="n">
         <v>3.611</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22" s="1" t="n">
         <v>1017</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" s="1" t="n">
         <v>836</v>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
+      <c r="J22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
+      <c r="L22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1" t="n">
         <v>0.004</v>
       </c>
-      <c r="N22" t="n">
+      <c r="N22" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="O22" t="n">
+      <c r="O22" s="1" t="n">
         <v>307</v>
       </c>
-      <c r="P22" t="n">
+      <c r="P22" s="1" t="n">
         <v>0.66</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="Q22" s="1" t="n">
         <v>621</v>
       </c>
-      <c r="R22" t="n">
+      <c r="R22" s="1" t="n">
         <v>426</v>
       </c>
-      <c r="S22" t="n">
+      <c r="S22" s="1" t="n">
         <v>0.41</v>
       </c>
-      <c r="T22" t="n">
+      <c r="T22" s="1" t="n">
         <v>174.11</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" s="1" t="n">
         <v>21.647</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="1" t="n">
         <v>0.076</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="1" t="n">
         <v>8295.063</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" s="1" t="n">
         <v>116.978</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23" s="1" t="n">
         <v>7189.359</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23" s="1" t="n">
         <v>117.513</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23" s="1" t="n">
         <v>2086</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23" s="1" t="n">
         <v>1701</v>
       </c>
-      <c r="J23" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" t="n">
+      <c r="J23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="L23" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" t="n">
+      <c r="L23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1" t="n">
         <v>0.002</v>
       </c>
-      <c r="N23" t="n">
+      <c r="N23" s="1" t="n">
         <v>323</v>
       </c>
-      <c r="O23" t="n">
+      <c r="O23" s="1" t="n">
         <v>631</v>
       </c>
-      <c r="P23" t="n">
+      <c r="P23" s="1" t="n">
         <v>0.66</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="Q23" s="1" t="n">
         <v>1258</v>
       </c>
-      <c r="R23" t="n">
+      <c r="R23" s="1" t="n">
         <v>868</v>
       </c>
-      <c r="S23" t="n">
+      <c r="S23" s="1" t="n">
         <v>0.41</v>
       </c>
-      <c r="T23" t="n">
+      <c r="T23" s="1" t="n">
         <v>178.34</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" s="1" t="n">
         <v>55.492</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="1" t="n">
         <v>4.254</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="1" t="n">
         <v>60077.688</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" s="1" t="n">
         <v>1509.916</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24" s="1" t="n">
         <v>57799.258</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24" s="1" t="n">
         <v>1500.238</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24" s="1" t="n">
         <v>4214</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24" s="1" t="n">
         <v>3417</v>
       </c>
-      <c r="J24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="n">
+      <c r="J24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1" t="n">
         <v>645</v>
       </c>
-      <c r="O24" t="n">
+      <c r="O24" s="1" t="n">
         <v>1276</v>
       </c>
-      <c r="P24" t="n">
+      <c r="P24" s="1" t="n">
         <v>0.66</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="Q24" s="1" t="n">
         <v>2521</v>
       </c>
-      <c r="R24" t="n">
+      <c r="R24" s="1" t="n">
         <v>1744</v>
       </c>
-      <c r="S24" t="n">
+      <c r="S24" s="1" t="n">
         <v>0.41</v>
       </c>
-      <c r="T24" t="n">
+      <c r="T24" s="1" t="n">
         <v>190.42</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="1" t="n">
         <v>119.869</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="1" t="n">
         <v>0.579</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="1" t="n">
         <v>398598.87</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" s="1" t="n">
         <v>5016.442</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25" s="1" t="n">
         <v>393987.734</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25" s="1" t="n">
         <v>5021.144</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25" s="1" t="n">
         <v>8457</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" s="1" t="n">
         <v>6832</v>
       </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
+      <c r="J25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="n">
+      <c r="L25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1" t="n">
         <v>1287</v>
       </c>
-      <c r="O25" t="n">
+      <c r="O25" s="1" t="n">
         <v>2562</v>
       </c>
-      <c r="P25" t="n">
+      <c r="P25" s="1" t="n">
         <v>0.67</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="Q25" s="1" t="n">
         <v>5034</v>
       </c>
-      <c r="R25" t="n">
+      <c r="R25" s="1" t="n">
         <v>3486</v>
       </c>
-      <c r="S25" t="n">
+      <c r="S25" s="1" t="n">
         <v>0.41</v>
       </c>
-      <c r="T25" t="n">
+      <c r="T25" s="1" t="n">
         <v>232.34</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" s="1" t="n">
         <v>196.868</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="1" t="n">
         <v>0.86</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="1" t="n">
         <v>3441425.874</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" s="1" t="n">
         <v>122883.464</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26" s="1" t="n">
         <v>3432076.115</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26" s="1" t="n">
         <v>122883.735</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26" s="1" t="n">
         <v>16927</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" s="1" t="n">
         <v>13642</v>
       </c>
-      <c r="J26" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="n">
+      <c r="J26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1" t="n">
         <v>2569</v>
       </c>
-      <c r="O26" t="n">
+      <c r="O26" s="1" t="n">
         <v>5129</v>
       </c>
-      <c r="P26" t="n">
+      <c r="P26" s="1" t="n">
         <v>0.67</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="Q26" s="1" t="n">
         <v>10045</v>
       </c>
-      <c r="R26" t="n">
+      <c r="R26" s="1" t="n">
         <v>6958</v>
       </c>
-      <c r="S26" t="n">
+      <c r="S26" s="1" t="n">
         <v>0.41</v>
       </c>
-      <c r="T26" t="n">
+      <c r="T26" s="1" t="n">
         <v>383.98</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
+      <c r="A27" s="1" t="inlineStr"/>
+      <c r="B27" s="1" t="inlineStr"/>
+      <c r="C27" s="1" t="inlineStr"/>
+      <c r="D27" s="1" t="inlineStr"/>
+      <c r="E27" s="1" t="inlineStr"/>
+      <c r="F27" s="1" t="inlineStr"/>
+      <c r="G27" s="1" t="inlineStr"/>
+      <c r="H27" s="1" t="inlineStr"/>
+      <c r="I27" s="1" t="inlineStr"/>
+      <c r="J27" s="1" t="inlineStr"/>
+      <c r="K27" s="1" t="inlineStr"/>
+      <c r="L27" s="1" t="inlineStr"/>
+      <c r="M27" s="1" t="inlineStr"/>
+      <c r="N27" s="1" t="inlineStr"/>
+      <c r="O27" s="1" t="inlineStr"/>
+      <c r="P27" s="1" t="inlineStr"/>
+      <c r="Q27" s="1" t="inlineStr"/>
+      <c r="R27" s="1" t="inlineStr"/>
+      <c r="S27" s="1" t="inlineStr"/>
+      <c r="T27" s="1" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr"/>
+      <c r="B28" s="1" t="inlineStr"/>
+      <c r="C28" s="1" t="inlineStr"/>
+      <c r="D28" s="1" t="inlineStr"/>
+      <c r="E28" s="1" t="inlineStr"/>
+      <c r="F28" s="1" t="inlineStr"/>
+      <c r="G28" s="1" t="inlineStr"/>
+      <c r="H28" s="1" t="inlineStr"/>
+      <c r="I28" s="1" t="inlineStr"/>
+      <c r="J28" s="1" t="inlineStr"/>
+      <c r="K28" s="1" t="inlineStr"/>
+      <c r="L28" s="1" t="inlineStr"/>
+      <c r="M28" s="1" t="inlineStr"/>
+      <c r="N28" s="1" t="inlineStr"/>
+      <c r="O28" s="1" t="inlineStr"/>
+      <c r="P28" s="1" t="inlineStr"/>
+      <c r="Q28" s="1" t="inlineStr"/>
+      <c r="R28" s="1" t="inlineStr"/>
+      <c r="S28" s="1" t="inlineStr"/>
+      <c r="T28" s="1" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Qsim: Algorithm = Amplitude Estimation Simulator = dm_simulator</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
+      <c r="E29" s="1" t="n"/>
+      <c r="F29" s="1" t="n"/>
+      <c r="G29" s="1" t="n"/>
+      <c r="H29" s="1" t="n"/>
+      <c r="I29" s="1" t="n"/>
+      <c r="J29" s="1" t="n"/>
+      <c r="K29" s="1" t="n"/>
+      <c r="L29" s="1" t="n"/>
+      <c r="M29" s="1" t="n"/>
+      <c r="N29" s="1" t="n"/>
+      <c r="O29" s="1" t="n"/>
+      <c r="P29" s="1" t="n"/>
+      <c r="Q29" s="1" t="n"/>
+      <c r="R29" s="1" t="n"/>
+      <c r="S29" s="1" t="n"/>
+      <c r="T29" s="1" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+      <c r="E30" s="1" t="n"/>
+      <c r="F30" s="1" t="n"/>
+      <c r="G30" s="1" t="n"/>
+      <c r="H30" s="1" t="n"/>
+      <c r="I30" s="1" t="n"/>
+      <c r="J30" s="1" t="n"/>
+      <c r="K30" s="1" t="n"/>
+      <c r="L30" s="1" t="n"/>
+      <c r="M30" s="1" t="n"/>
+      <c r="N30" s="1" t="n"/>
+      <c r="O30" s="1" t="n"/>
+      <c r="P30" s="1" t="n"/>
+      <c r="Q30" s="1" t="n"/>
+      <c r="R30" s="1" t="n"/>
+      <c r="S30" s="1" t="n"/>
+      <c r="T30" s="1" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 4 Max_Qubits = 10 Skip_Qubits = 1 num_circuits = 2  QV_ = None Last_Updated = 2025-02-10 11:55:00</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="n"/>
+      <c r="C31" s="1" t="n"/>
+      <c r="D31" s="1" t="n"/>
+      <c r="E31" s="1" t="n"/>
+      <c r="F31" s="1" t="n"/>
+      <c r="G31" s="1" t="n"/>
+      <c r="H31" s="1" t="n"/>
+      <c r="I31" s="1" t="n"/>
+      <c r="J31" s="1" t="n"/>
+      <c r="K31" s="1" t="n"/>
+      <c r="L31" s="1" t="n"/>
+      <c r="M31" s="1" t="n"/>
+      <c r="N31" s="1" t="n"/>
+      <c r="O31" s="1" t="n"/>
+      <c r="P31" s="1" t="n"/>
+      <c r="Q31" s="1" t="n"/>
+      <c r="R31" s="1" t="n"/>
+      <c r="S31" s="1" t="n"/>
+      <c r="T31" s="1" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>max_memory (MB)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" t="n">
+        <v>110.604</v>
+      </c>
+      <c r="C33" t="n">
+        <v>28.004</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2543.473</v>
+      </c>
+      <c r="E33" t="n">
+        <v>643.704</v>
+      </c>
+      <c r="F33" t="n">
+        <v>14.002</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="H33" t="n">
+        <v>208</v>
+      </c>
+      <c r="I33" t="n">
+        <v>167.5</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>37</v>
+      </c>
+      <c r="O33" t="n">
+        <v>62</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>128.5</v>
+      </c>
+      <c r="R33" t="n">
+        <v>85</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T33" t="n">
+        <v>169.5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>5</v>
+      </c>
+      <c r="B34" t="n">
+        <v>7.714</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="D34" t="n">
+        <v>326.915</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="F34" t="n">
+        <v>50.646</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="H34" t="n">
+        <v>479</v>
+      </c>
+      <c r="I34" t="n">
+        <v>363</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>79</v>
+      </c>
+      <c r="O34" t="n">
+        <v>144</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>277</v>
+      </c>
+      <c r="R34" t="n">
+        <v>188</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T34" t="n">
+        <v>170.84</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>6</v>
+      </c>
+      <c r="B35" t="n">
+        <v>12.003</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="D35" t="n">
+        <v>984.596</v>
+      </c>
+      <c r="E35" t="n">
+        <v>7.997</v>
+      </c>
+      <c r="F35" t="n">
+        <v>461.558</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1017</v>
+      </c>
+      <c r="I35" t="n">
+        <v>836</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>161</v>
+      </c>
+      <c r="O35" t="n">
+        <v>307</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>621</v>
+      </c>
+      <c r="R35" t="n">
+        <v>426</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T35" t="n">
+        <v>173.34</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>7</v>
+      </c>
+      <c r="B36" t="n">
+        <v>21.329</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>4629.913</v>
+      </c>
+      <c r="E36" t="n">
+        <v>15.501</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3570.347</v>
+      </c>
+      <c r="G36" t="n">
+        <v>9.882999999999999</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2086</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1701</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N36" t="n">
+        <v>323</v>
+      </c>
+      <c r="O36" t="n">
+        <v>631</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1258</v>
+      </c>
+      <c r="R36" t="n">
+        <v>868</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T36" t="n">
+        <v>177.37</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>8</v>
+      </c>
+      <c r="B37" t="n">
+        <v>68.711</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="D37" t="n">
+        <v>31408.188</v>
+      </c>
+      <c r="E37" t="n">
+        <v>151.431</v>
+      </c>
+      <c r="F37" t="n">
+        <v>29239.596</v>
+      </c>
+      <c r="G37" t="n">
+        <v>153.081</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4214</v>
+      </c>
+      <c r="I37" t="n">
+        <v>3417</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="N37" t="n">
+        <v>645</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1276</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>2521</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1744</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T37" t="n">
+        <v>189.78</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>9</v>
+      </c>
+      <c r="B38" t="n">
+        <v>108.442</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="D38" t="n">
+        <v>243110.663</v>
+      </c>
+      <c r="E38" t="n">
+        <v>122.646</v>
+      </c>
+      <c r="F38" t="n">
+        <v>238635.866</v>
+      </c>
+      <c r="G38" t="n">
+        <v>69.383</v>
+      </c>
+      <c r="H38" t="n">
+        <v>8457</v>
+      </c>
+      <c r="I38" t="n">
+        <v>6832</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N38" t="n">
+        <v>1287</v>
+      </c>
+      <c r="O38" t="n">
+        <v>2562</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>5034</v>
+      </c>
+      <c r="R38" t="n">
+        <v>3486</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T38" t="n">
+        <v>231.02</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>10</v>
+      </c>
+      <c r="B39" t="n">
+        <v>188.401</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1.755</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2093656.623</v>
+      </c>
+      <c r="E39" t="n">
+        <v>905.23</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2084767.013</v>
+      </c>
+      <c r="G39" t="n">
+        <v>876.811</v>
+      </c>
+      <c r="H39" t="n">
+        <v>16927</v>
+      </c>
+      <c r="I39" t="n">
+        <v>13642</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N39" t="n">
+        <v>2569</v>
+      </c>
+      <c r="O39" t="n">
+        <v>5129</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>10045</v>
+      </c>
+      <c r="R39" t="n">
+        <v>6958</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T39" t="n">
+        <v>382.17</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
     <mergeCell ref="A16:S16"/>
     <mergeCell ref="A17:S17"/>
     <mergeCell ref="A18:S18"/>
+    <mergeCell ref="A29:S29"/>
+    <mergeCell ref="A31:S31"/>
     <mergeCell ref="A3:S3"/>
     <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A30:S30"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A15:S15"/>
   </mergeCells>

</xml_diff>